<commit_message>
graficas actualizadas en excel
</commit_message>
<xml_diff>
--- a/Data_analysis/Data_analysis.xlsx
+++ b/Data_analysis/Data_analysis.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20399"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{905A694A-0A5E-4D03-92EB-B290E6A69642}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D7DD466-D83D-450C-9779-669326A45FB5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5580" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6510" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="candados" sheetId="1" r:id="rId1"/>
@@ -8090,66 +8090,66 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>pattern!$B$3:$B$10</c:f>
+              <c:f>mandrill!$B$3:$B$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>59.960999999999999</c:v>
+                  <c:v>47.631999999999998</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>76.299000000000007</c:v>
+                  <c:v>80.001999999999995</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>80.724999999999994</c:v>
+                  <c:v>88.1</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>84.954999999999998</c:v>
+                  <c:v>92.644999999999996</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>88.144999999999996</c:v>
+                  <c:v>95.164000000000001</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>89.966999999999999</c:v>
+                  <c:v>96.268000000000001</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>93.807000000000002</c:v>
+                  <c:v>97.706000000000003</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>95.89</c:v>
+                  <c:v>98.563999999999993</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>pattern!$A$3:$A$10</c:f>
+              <c:f>mandrill!$A$3:$A$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>0.54688000000000003</c:v>
+                  <c:v>5.8864000000000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>27.780999999999999</c:v>
+                  <c:v>73.400000000000006</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>36.609000000000002</c:v>
+                  <c:v>129.86000000000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>270.2</c:v>
+                  <c:v>197.33</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>869.44</c:v>
+                  <c:v>265.89999999999998</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1479.8</c:v>
+                  <c:v>317.36</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6031.1</c:v>
+                  <c:v>455.02</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>6980</c:v>
+                  <c:v>698.92</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8193,66 +8193,66 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>pattern!$G$3:$G$10</c:f>
+              <c:f>mandrill!$G$3:$G$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>69.28</c:v>
+                  <c:v>50.875999999999998</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>78.72</c:v>
+                  <c:v>80.656999999999996</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>82.424999999999997</c:v>
+                  <c:v>88.245999999999995</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>86.915999999999997</c:v>
+                  <c:v>92.784999999999997</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>90.108999999999995</c:v>
+                  <c:v>95.412999999999997</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>92.061000000000007</c:v>
+                  <c:v>96.587000000000003</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>95.968000000000004</c:v>
+                  <c:v>98.13</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>98.713999999999999</c:v>
+                  <c:v>99.025999999999996</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>pattern!$F$3:$F$10</c:f>
+              <c:f>mandrill!$F$3:$F$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>0.54688000000000003</c:v>
+                  <c:v>5.8864000000000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>27.780999999999999</c:v>
+                  <c:v>73.400000000000006</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>36.609000000000002</c:v>
+                  <c:v>129.86000000000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>270.2</c:v>
+                  <c:v>197.33</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>869.44</c:v>
+                  <c:v>265.89999999999998</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1479.8</c:v>
+                  <c:v>317.36</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6031.1</c:v>
+                  <c:v>455.02</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>6980</c:v>
+                  <c:v>698.92</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8279,7 +8279,8 @@
         <c:axId val="2085306543"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:min val="55"/>
+          <c:max val="110"/>
+          <c:min val="40"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -8698,66 +8699,66 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>pattern!$B$3:$B$10</c:f>
+              <c:f>mandrill!$B$3:$B$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>59.960999999999999</c:v>
+                  <c:v>47.631999999999998</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>76.299000000000007</c:v>
+                  <c:v>80.001999999999995</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>80.724999999999994</c:v>
+                  <c:v>88.1</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>84.954999999999998</c:v>
+                  <c:v>92.644999999999996</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>88.144999999999996</c:v>
+                  <c:v>95.164000000000001</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>89.966999999999999</c:v>
+                  <c:v>96.268000000000001</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>93.807000000000002</c:v>
+                  <c:v>97.706000000000003</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>95.89</c:v>
+                  <c:v>98.563999999999993</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>pattern!$C$3:$C$10</c:f>
+              <c:f>mandrill!$C$3:$C$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>47.003999999999998</c:v>
+                  <c:v>35.122999999999998</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>29.945</c:v>
+                  <c:v>24.164000000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>28.747</c:v>
+                  <c:v>21.687000000000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>20.065999999999999</c:v>
+                  <c:v>19.869</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>14.99</c:v>
+                  <c:v>18.574000000000002</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>12.680999999999999</c:v>
+                  <c:v>17.806000000000001</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6.5787000000000004</c:v>
+                  <c:v>16.241</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>5.9440999999999997</c:v>
+                  <c:v>14.377000000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8801,66 +8802,66 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>pattern!$G$3:$G$10</c:f>
+              <c:f>mandrill!$G$3:$G$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>69.28</c:v>
+                  <c:v>50.875999999999998</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>78.72</c:v>
+                  <c:v>80.656999999999996</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>82.424999999999997</c:v>
+                  <c:v>88.245999999999995</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>86.915999999999997</c:v>
+                  <c:v>92.784999999999997</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>90.108999999999995</c:v>
+                  <c:v>95.412999999999997</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>92.061000000000007</c:v>
+                  <c:v>96.587000000000003</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>95.968000000000004</c:v>
+                  <c:v>98.13</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>98.713999999999999</c:v>
+                  <c:v>99.025999999999996</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>pattern!$H$3:$H$10</c:f>
+              <c:f>mandrill!$H$3:$H$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>47.003999999999998</c:v>
+                  <c:v>35.122999999999998</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>29.945</c:v>
+                  <c:v>24.164000000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>28.747</c:v>
+                  <c:v>21.687000000000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>20.065999999999999</c:v>
+                  <c:v>19.869</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>14.99</c:v>
+                  <c:v>18.574000000000002</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>12.680999999999999</c:v>
+                  <c:v>17.806000000000001</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6.5787000000000004</c:v>
+                  <c:v>16.241</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>5.9440999999999997</c:v>
+                  <c:v>14.377000000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8887,7 +8888,7 @@
         <c:axId val="2085306543"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:min val="55"/>
+          <c:min val="40"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -25701,15 +25702,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>590550</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:colOff>561975</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>285750</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:colOff>257175</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -25781,16 +25782,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>152400</xdr:colOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>523875</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>533400</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
+      <xdr:colOff>285750</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -25863,15 +25864,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>104775</xdr:colOff>
+      <xdr:colOff>47625</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>485775</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
+      <xdr:colOff>390525</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -25945,14 +25946,14 @@
     <xdr:from>
       <xdr:col>10</xdr:col>
       <xdr:colOff>333375</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
       <xdr:colOff>28575</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -26024,16 +26025,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>57149</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>57151</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>600074</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>180976</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>400050</xdr:colOff>
+      <xdr:colOff>295275</xdr:colOff>
       <xdr:row>31</xdr:row>
-      <xdr:rowOff>57151</xdr:rowOff>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -26107,14 +26108,14 @@
     <xdr:from>
       <xdr:col>11</xdr:col>
       <xdr:colOff>171450</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>57149</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>514351</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>85724</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -26187,15 +26188,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:colOff>19051</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>47624</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>342901</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:colOff>361951</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>38099</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -26268,15 +26269,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>228600</xdr:colOff>
+      <xdr:colOff>228601</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>76199</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>571501</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:colOff>552451</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>66674</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -26348,16 +26349,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>590550</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>361950</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -26430,15 +26431,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>200025</xdr:colOff>
+      <xdr:colOff>238125</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>581025</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -26510,16 +26511,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>38100</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>590550</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>419100</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:colOff>333375</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -30785,7 +30786,7 @@
   <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L19" sqref="L19"/>
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -30832,210 +30833,210 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>0.54688000000000003</v>
+        <v>5.8864000000000001</v>
       </c>
       <c r="B3">
-        <v>59.960999999999999</v>
+        <v>47.631999999999998</v>
       </c>
       <c r="C3">
-        <v>47.003999999999998</v>
+        <v>35.122999999999998</v>
       </c>
       <c r="D3">
-        <v>0.99997999999999998</v>
+        <v>0.99594000000000005</v>
       </c>
       <c r="F3">
-        <v>0.54688000000000003</v>
+        <v>5.8864000000000001</v>
       </c>
       <c r="G3">
-        <v>69.28</v>
+        <v>50.875999999999998</v>
       </c>
       <c r="H3">
-        <v>47.003999999999998</v>
+        <v>35.122999999999998</v>
       </c>
       <c r="I3">
-        <v>0.99997999999999998</v>
+        <v>0.99594000000000005</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>27.780999999999999</v>
+        <v>73.400000000000006</v>
       </c>
       <c r="B4">
-        <v>76.299000000000007</v>
+        <v>80.001999999999995</v>
       </c>
       <c r="C4">
-        <v>29.945</v>
+        <v>24.164000000000001</v>
       </c>
       <c r="D4">
-        <v>0.99909000000000003</v>
+        <v>0.95430999999999999</v>
       </c>
       <c r="F4">
-        <v>27.780999999999999</v>
+        <v>73.400000000000006</v>
       </c>
       <c r="G4">
-        <v>78.72</v>
+        <v>80.656999999999996</v>
       </c>
       <c r="H4">
-        <v>29.945</v>
+        <v>24.164000000000001</v>
       </c>
       <c r="I4">
-        <v>0.99909000000000003</v>
+        <v>0.95430999999999999</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>36.609000000000002</v>
+        <v>129.86000000000001</v>
       </c>
       <c r="B5">
-        <v>80.724999999999994</v>
+        <v>88.1</v>
       </c>
       <c r="C5">
-        <v>28.747</v>
+        <v>21.687000000000001</v>
       </c>
       <c r="D5">
-        <v>0.99882000000000004</v>
+        <v>0.92457</v>
       </c>
       <c r="F5">
-        <v>36.609000000000002</v>
+        <v>129.86000000000001</v>
       </c>
       <c r="G5">
-        <v>82.424999999999997</v>
+        <v>88.245999999999995</v>
       </c>
       <c r="H5">
-        <v>28.747</v>
+        <v>21.687000000000001</v>
       </c>
       <c r="I5">
-        <v>0.99882000000000004</v>
+        <v>0.92457</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>270.2</v>
+        <v>197.33</v>
       </c>
       <c r="B6">
-        <v>84.954999999999998</v>
+        <v>92.644999999999996</v>
       </c>
       <c r="C6">
-        <v>20.065999999999999</v>
+        <v>19.869</v>
       </c>
       <c r="D6">
-        <v>0.99084000000000005</v>
+        <v>0.89093</v>
       </c>
       <c r="F6">
-        <v>270.2</v>
+        <v>197.33</v>
       </c>
       <c r="G6">
-        <v>86.915999999999997</v>
+        <v>92.784999999999997</v>
       </c>
       <c r="H6">
-        <v>20.065999999999999</v>
+        <v>19.869</v>
       </c>
       <c r="I6">
-        <v>0.99084000000000005</v>
+        <v>0.89093</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>869.44</v>
+        <v>265.89999999999998</v>
       </c>
       <c r="B7">
-        <v>88.144999999999996</v>
+        <v>95.164000000000001</v>
       </c>
       <c r="C7">
-        <v>14.99</v>
+        <v>18.574000000000002</v>
       </c>
       <c r="D7">
-        <v>0.96897</v>
+        <v>0.85538000000000003</v>
       </c>
       <c r="F7">
-        <v>869.44</v>
+        <v>265.89999999999998</v>
       </c>
       <c r="G7">
-        <v>90.108999999999995</v>
+        <v>95.412999999999997</v>
       </c>
       <c r="H7">
-        <v>14.99</v>
+        <v>18.574000000000002</v>
       </c>
       <c r="I7">
-        <v>0.96897</v>
+        <v>0.85538000000000003</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>1479.8</v>
+        <v>317.36</v>
       </c>
       <c r="B8">
-        <v>89.966999999999999</v>
+        <v>96.268000000000001</v>
       </c>
       <c r="C8">
-        <v>12.680999999999999</v>
+        <v>17.806000000000001</v>
       </c>
       <c r="D8">
-        <v>0.94593000000000005</v>
+        <v>0.82913000000000003</v>
       </c>
       <c r="F8">
-        <v>1479.8</v>
+        <v>317.36</v>
       </c>
       <c r="G8">
-        <v>92.061000000000007</v>
+        <v>96.587000000000003</v>
       </c>
       <c r="H8">
-        <v>12.680999999999999</v>
+        <v>17.806000000000001</v>
       </c>
       <c r="I8">
-        <v>0.94593000000000005</v>
+        <v>0.82913000000000003</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>6031.1</v>
+        <v>455.02</v>
       </c>
       <c r="B9">
-        <v>93.807000000000002</v>
+        <v>97.706000000000003</v>
       </c>
       <c r="C9">
-        <v>6.5787000000000004</v>
+        <v>16.241</v>
       </c>
       <c r="D9">
-        <v>0.74150000000000005</v>
+        <v>0.76197999999999999</v>
       </c>
       <c r="F9">
-        <v>6031.1</v>
+        <v>455.02</v>
       </c>
       <c r="G9">
-        <v>95.968000000000004</v>
+        <v>98.13</v>
       </c>
       <c r="H9">
-        <v>6.5787000000000004</v>
+        <v>16.241</v>
       </c>
       <c r="I9">
-        <v>0.74150000000000005</v>
+        <v>0.76197999999999999</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>6980</v>
+        <v>698.92</v>
       </c>
       <c r="B10">
-        <v>95.89</v>
+        <v>98.563999999999993</v>
       </c>
       <c r="C10">
-        <v>5.9440999999999997</v>
+        <v>14.377000000000001</v>
       </c>
       <c r="D10">
-        <v>0.71897</v>
+        <v>0.63966000000000001</v>
       </c>
       <c r="F10">
-        <v>6980</v>
+        <v>698.92</v>
       </c>
       <c r="G10">
-        <v>98.713999999999999</v>
+        <v>99.025999999999996</v>
       </c>
       <c r="H10">
-        <v>5.9440999999999997</v>
+        <v>14.377000000000001</v>
       </c>
       <c r="I10">
-        <v>0.71897</v>
+        <v>0.63966000000000001</v>
       </c>
     </row>
   </sheetData>
@@ -31860,7 +31861,7 @@
   <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="R24" sqref="R24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -32398,7 +32399,7 @@
   <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I3" sqref="I3:I10"/>
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -32667,7 +32668,7 @@
   <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3:D10"/>
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>